<commit_message>
Fix minor issues, fix timer code (now works)
</commit_message>
<xml_diff>
--- a/SaveSignal/Signals.xlsx
+++ b/SaveSignal/Signals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VGU\2nd Year\Semester 2\IoT and Smart Devices\AC Remote Control Project\ARDUINO\SaveSignal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VGU\2nd Year\Semester 2\IOT - IoT and Smart Devices\AC Remote Control Project\ARDUINO\SaveSignal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C422BF8-9929-4D27-ABE5-E071F6AA2E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DCB219-B308-42B1-814F-49A462F73F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1383,7 +1383,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1405,11 +1405,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFDAE3E3"/>
-      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1447,14 +1442,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1746,32 +1738,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G145"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BH65" sqref="BH65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.399999999999999"/>
+  <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="15.734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.26171875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26171875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26171875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.41796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.3125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.20703125" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.3671875" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1787,17 +1781,17 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="6">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A2" s="5">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="str">
+      <c r="D2" s="6" t="str">
         <f>CONCATENATE("_",A2,"_",B2,"_",C2)</f>
         <v>_25_Top_Low</v>
       </c>
@@ -1819,17 +1813,17 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="7">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A3" s="6">
         <v>25</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="str">
+      <c r="D3" s="6" t="str">
         <f t="shared" ref="D3:D66" si="0">CONCATENATE("_",A3,"_",B3,"_",C3)</f>
         <v>_25_Top_Medium</v>
       </c>
@@ -1844,24 +1838,24 @@
         <v>160</v>
       </c>
       <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:I66" si="2">CONCATENATE("{",$H$1,D3,$H$1,", ",D3,"},")</f>
+        <f t="shared" ref="H3:H66" si="2">CONCATENATE("{",$H$1,D3,$H$1,", ",D3,"},")</f>
         <v>{"_25_Top_Medium", _25_Top_Medium},</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="7">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A4" s="6">
         <v>25</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="str">
+      <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Top_High</v>
       </c>
@@ -1883,17 +1877,17 @@
         <v>305</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="7">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A5" s="6">
         <v>25</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="str">
+      <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Top_Auto</v>
       </c>
@@ -1915,17 +1909,17 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="7">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A6" s="6">
         <v>25</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="str">
+      <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_High_Low</v>
       </c>
@@ -1947,17 +1941,17 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A7" s="6">
         <v>25</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7" t="str">
+      <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_High_Medium</v>
       </c>
@@ -1979,17 +1973,17 @@
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="7">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A8" s="6">
         <v>25</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7" t="str">
+      <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_High_High</v>
       </c>
@@ -2011,17 +2005,17 @@
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="7">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A9" s="6">
         <v>25</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="7" t="str">
+      <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_High_Auto</v>
       </c>
@@ -2043,17 +2037,17 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="7">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A10" s="6">
         <v>25</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="7" t="str">
+      <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Mid_Low</v>
       </c>
@@ -2075,17 +2069,17 @@
         <v>311</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="7">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A11" s="6">
         <v>25</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="7" t="str">
+      <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Mid_Medium</v>
       </c>
@@ -2107,17 +2101,17 @@
         <v>312</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="7">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A12" s="6">
         <v>25</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="7" t="str">
+      <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Mid_High</v>
       </c>
@@ -2139,17 +2133,17 @@
         <v>313</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="7">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A13" s="6">
         <v>25</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="7" t="str">
+      <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Mid_Auto</v>
       </c>
@@ -2171,17 +2165,17 @@
         <v>314</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="7">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A14" s="6">
         <v>25</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="7" t="str">
+      <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Low_Low</v>
       </c>
@@ -2203,17 +2197,17 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="7">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A15" s="6">
         <v>25</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="7" t="str">
+      <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Low_Medium</v>
       </c>
@@ -2235,17 +2229,17 @@
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="7">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A16" s="6">
         <v>25</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="7" t="str">
+      <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Low_High</v>
       </c>
@@ -2267,17 +2261,17 @@
         <v>317</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="7">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A17" s="6">
         <v>25</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="7" t="str">
+      <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Low_Auto</v>
       </c>
@@ -2299,17 +2293,17 @@
         <v>318</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="7">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A18" s="6">
         <v>25</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="7" t="str">
+      <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Bottom_Low</v>
       </c>
@@ -2331,17 +2325,17 @@
         <v>319</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="7">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A19" s="6">
         <v>25</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="7" t="str">
+      <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Bottom_Medium</v>
       </c>
@@ -2363,17 +2357,17 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="7">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A20" s="6">
         <v>25</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="7" t="str">
+      <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Bottom_High</v>
       </c>
@@ -2395,17 +2389,17 @@
         <v>321</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="7">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A21" s="6">
         <v>25</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="7" t="str">
+      <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Bottom_Auto</v>
       </c>
@@ -2427,17 +2421,17 @@
         <v>322</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="7">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A22" s="6">
         <v>25</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="7" t="str">
+      <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Auto_Low</v>
       </c>
@@ -2459,17 +2453,17 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="7">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A23" s="6">
         <v>25</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="7" t="str">
+      <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Auto_Medium</v>
       </c>
@@ -2491,17 +2485,17 @@
         <v>324</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="7">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A24" s="6">
         <v>25</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="7" t="str">
+      <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Auto_High</v>
       </c>
@@ -2523,17 +2517,17 @@
         <v>325</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="7">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A25" s="6">
         <v>25</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="7" t="str">
+      <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_25_Auto_Auto</v>
       </c>
@@ -2555,17 +2549,17 @@
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="7">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A26" s="6">
         <v>26</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="7" t="str">
+      <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Top_Low</v>
       </c>
@@ -2587,17 +2581,17 @@
         <v>327</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="7">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="7" t="str">
+      <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Top_Medium</v>
       </c>
@@ -2619,17 +2613,17 @@
         <v>328</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="7">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A28" s="6">
         <v>26</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="7" t="str">
+      <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Top_High</v>
       </c>
@@ -2651,17 +2645,17 @@
         <v>329</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="7">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A29" s="6">
         <v>26</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="7" t="str">
+      <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Top_Auto</v>
       </c>
@@ -2683,17 +2677,17 @@
         <v>330</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="7">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A30" s="6">
         <v>26</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="7" t="str">
+      <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_High_Low</v>
       </c>
@@ -2715,17 +2709,17 @@
         <v>331</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="7">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A31" s="6">
         <v>26</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="7" t="str">
+      <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_High_Medium</v>
       </c>
@@ -2747,17 +2741,17 @@
         <v>332</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="7">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A32" s="6">
         <v>26</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="7" t="str">
+      <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_High_High</v>
       </c>
@@ -2779,17 +2773,17 @@
         <v>333</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="7">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A33" s="6">
         <v>26</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="7" t="str">
+      <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_High_Auto</v>
       </c>
@@ -2811,17 +2805,17 @@
         <v>334</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="7">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A34" s="6">
         <v>26</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="7" t="str">
+      <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Mid_Low</v>
       </c>
@@ -2843,17 +2837,17 @@
         <v>335</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="7">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A35" s="6">
         <v>26</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="7" t="str">
+      <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Mid_Medium</v>
       </c>
@@ -2875,17 +2869,17 @@
         <v>336</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="7">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A36" s="6">
         <v>26</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="7" t="str">
+      <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Mid_High</v>
       </c>
@@ -2907,21 +2901,21 @@
         <v>337</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="7">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A37" s="6">
         <v>26</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="7" t="str">
+      <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Mid_Auto</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F37" s="1" t="str">
@@ -2939,17 +2933,17 @@
         <v>338</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="7">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A38" s="6">
         <v>26</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="7" t="str">
+      <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Low_Low</v>
       </c>
@@ -2971,17 +2965,17 @@
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="7">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A39" s="6">
         <v>26</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="7" t="str">
+      <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Low_Medium</v>
       </c>
@@ -3003,17 +2997,17 @@
         <v>340</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="7">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A40" s="6">
         <v>26</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="7" t="str">
+      <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Low_High</v>
       </c>
@@ -3035,17 +3029,17 @@
         <v>341</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="7">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A41" s="6">
         <v>26</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="7" t="str">
+      <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Low_Auto</v>
       </c>
@@ -3067,17 +3061,17 @@
         <v>342</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="7">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A42" s="6">
         <v>26</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="7" t="str">
+      <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Bottom_Low</v>
       </c>
@@ -3099,17 +3093,17 @@
         <v>343</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="7">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A43" s="6">
         <v>26</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="7" t="str">
+      <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Bottom_Medium</v>
       </c>
@@ -3131,17 +3125,17 @@
         <v>344</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="7">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A44" s="6">
         <v>26</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="7" t="str">
+      <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Bottom_High</v>
       </c>
@@ -3163,17 +3157,17 @@
         <v>345</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="7">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A45" s="6">
         <v>26</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="7" t="str">
+      <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Bottom_Auto</v>
       </c>
@@ -3195,17 +3189,17 @@
         <v>346</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="7">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A46" s="6">
         <v>26</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="7" t="str">
+      <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Auto_Low</v>
       </c>
@@ -3227,17 +3221,17 @@
         <v>347</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="7">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A47" s="6">
         <v>26</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="7" t="str">
+      <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Auto_Medium</v>
       </c>
@@ -3259,17 +3253,17 @@
         <v>348</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="7">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A48" s="6">
         <v>26</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="7" t="str">
+      <c r="D48" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Auto_High</v>
       </c>
@@ -3291,17 +3285,17 @@
         <v>349</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="7">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A49" s="6">
         <v>26</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="7" t="str">
+      <c r="D49" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_26_Auto_Auto</v>
       </c>
@@ -3323,17 +3317,17 @@
         <v>350</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="7">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A50" s="6">
         <v>27</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="7" t="str">
+      <c r="D50" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Top_Low</v>
       </c>
@@ -3355,17 +3349,17 @@
         <v>351</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="7">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A51" s="6">
         <v>27</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="7" t="str">
+      <c r="D51" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Top_Medium</v>
       </c>
@@ -3387,17 +3381,17 @@
         <v>352</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="7">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A52" s="6">
         <v>27</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="7" t="str">
+      <c r="D52" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Top_High</v>
       </c>
@@ -3419,17 +3413,17 @@
         <v>353</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="7">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A53" s="6">
         <v>27</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="7" t="str">
+      <c r="D53" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Top_Auto</v>
       </c>
@@ -3451,17 +3445,17 @@
         <v>354</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="7">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A54" s="6">
         <v>27</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="7" t="str">
+      <c r="D54" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_High_Low</v>
       </c>
@@ -3483,17 +3477,17 @@
         <v>355</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="7">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A55" s="6">
         <v>27</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="7" t="str">
+      <c r="D55" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_High_Medium</v>
       </c>
@@ -3515,17 +3509,17 @@
         <v>356</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="7">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A56" s="6">
         <v>27</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="7" t="str">
+      <c r="D56" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_High_High</v>
       </c>
@@ -3547,17 +3541,17 @@
         <v>357</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="7">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A57" s="6">
         <v>27</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="7" t="str">
+      <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_High_Auto</v>
       </c>
@@ -3579,17 +3573,17 @@
         <v>358</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="7">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A58" s="6">
         <v>27</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="7" t="str">
+      <c r="D58" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Mid_Low</v>
       </c>
@@ -3611,17 +3605,17 @@
         <v>359</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="7">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A59" s="6">
         <v>27</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="7" t="str">
+      <c r="D59" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Mid_Medium</v>
       </c>
@@ -3643,17 +3637,17 @@
         <v>360</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="7">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A60" s="6">
         <v>27</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="7" t="str">
+      <c r="D60" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Mid_High</v>
       </c>
@@ -3675,17 +3669,17 @@
         <v>361</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="7">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A61" s="6">
         <v>27</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="7" t="str">
+      <c r="D61" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Mid_Auto</v>
       </c>
@@ -3707,17 +3701,17 @@
         <v>362</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="7">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A62" s="6">
         <v>27</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="7" t="str">
+      <c r="D62" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Low_Low</v>
       </c>
@@ -3739,17 +3733,17 @@
         <v>363</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="7">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A63" s="6">
         <v>27</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="7" t="str">
+      <c r="D63" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Low_Medium</v>
       </c>
@@ -3771,17 +3765,17 @@
         <v>364</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="7">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A64" s="6">
         <v>27</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="7" t="str">
+      <c r="D64" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Low_High</v>
       </c>
@@ -3803,17 +3797,17 @@
         <v>365</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="7">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A65" s="6">
         <v>27</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D65" s="7" t="str">
+      <c r="D65" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Low_Auto</v>
       </c>
@@ -3835,17 +3829,17 @@
         <v>366</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="7">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A66" s="6">
         <v>27</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="7" t="str">
+      <c r="D66" s="6" t="str">
         <f t="shared" si="0"/>
         <v>_27_Bottom_Low</v>
       </c>
@@ -3867,17 +3861,17 @@
         <v>367</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="7">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A67" s="6">
         <v>27</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="7" t="str">
+      <c r="D67" s="6" t="str">
         <f t="shared" ref="D67:D130" si="3">CONCATENATE("_",A67,"_",B67,"_",C67)</f>
         <v>_27_Bottom_Medium</v>
       </c>
@@ -3892,24 +3886,24 @@
         <v>224</v>
       </c>
       <c r="H67" s="1" t="str">
-        <f t="shared" ref="H67:I130" si="5">CONCATENATE("{",$H$1,D67,$H$1,", ",D67,"},")</f>
+        <f t="shared" ref="H67:H130" si="5">CONCATENATE("{",$H$1,D67,$H$1,", ",D67,"},")</f>
         <v>{"_27_Bottom_Medium", _27_Bottom_Medium},</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="7">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A68" s="6">
         <v>27</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="7" t="str">
+      <c r="D68" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_27_Bottom_High</v>
       </c>
@@ -3931,17 +3925,17 @@
         <v>369</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="7">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A69" s="6">
         <v>27</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="7" t="str">
+      <c r="D69" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_27_Bottom_Auto</v>
       </c>
@@ -3963,17 +3957,17 @@
         <v>370</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="7">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A70" s="6">
         <v>27</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="7" t="str">
+      <c r="D70" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_27_Auto_Low</v>
       </c>
@@ -3995,17 +3989,17 @@
         <v>371</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="7">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A71" s="6">
         <v>27</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C71" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D71" s="7" t="str">
+      <c r="D71" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_27_Auto_Medium</v>
       </c>
@@ -4027,17 +4021,17 @@
         <v>372</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="7">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A72" s="6">
         <v>27</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D72" s="7" t="str">
+      <c r="D72" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_27_Auto_High</v>
       </c>
@@ -4059,17 +4053,17 @@
         <v>373</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="7">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A73" s="6">
         <v>27</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="7" t="str">
+      <c r="D73" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_27_Auto_Auto</v>
       </c>
@@ -4091,17 +4085,17 @@
         <v>374</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="7">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A74" s="6">
         <v>28</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C74" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="7" t="str">
+      <c r="D74" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Top_Low</v>
       </c>
@@ -4123,17 +4117,17 @@
         <v>375</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="7">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A75" s="6">
         <v>28</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B75" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="C75" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D75" s="7" t="str">
+      <c r="D75" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Top_Medium</v>
       </c>
@@ -4155,17 +4149,17 @@
         <v>376</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="7">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A76" s="6">
         <v>28</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D76" s="7" t="str">
+      <c r="D76" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Top_High</v>
       </c>
@@ -4187,17 +4181,17 @@
         <v>377</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
-      <c r="A77" s="7">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A77" s="6">
         <v>28</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="7" t="str">
+      <c r="D77" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Top_Auto</v>
       </c>
@@ -4219,17 +4213,17 @@
         <v>378</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="7">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A78" s="6">
         <v>28</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D78" s="7" t="str">
+      <c r="D78" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_High_Low</v>
       </c>
@@ -4251,17 +4245,17 @@
         <v>379</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="7">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A79" s="6">
         <v>28</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B79" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C79" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D79" s="7" t="str">
+      <c r="D79" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_High_Medium</v>
       </c>
@@ -4283,17 +4277,17 @@
         <v>380</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="7">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A80" s="6">
         <v>28</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D80" s="7" t="str">
+      <c r="D80" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_High_High</v>
       </c>
@@ -4315,17 +4309,17 @@
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="7">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A81" s="6">
         <v>28</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B81" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C81" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D81" s="7" t="str">
+      <c r="D81" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_High_Auto</v>
       </c>
@@ -4347,17 +4341,17 @@
         <v>382</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="7">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A82" s="6">
         <v>28</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C82" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D82" s="7" t="str">
+      <c r="D82" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Mid_Low</v>
       </c>
@@ -4379,17 +4373,17 @@
         <v>383</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="7">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A83" s="6">
         <v>28</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C83" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="7" t="str">
+      <c r="D83" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Mid_Medium</v>
       </c>
@@ -4411,17 +4405,17 @@
         <v>384</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="7">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A84" s="6">
         <v>28</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B84" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C84" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D84" s="7" t="str">
+      <c r="D84" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Mid_High</v>
       </c>
@@ -4443,17 +4437,17 @@
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="7">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A85" s="6">
         <v>28</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B85" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="7" t="str">
+      <c r="D85" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Mid_Auto</v>
       </c>
@@ -4475,17 +4469,17 @@
         <v>386</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="7">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A86" s="6">
         <v>28</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="B86" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D86" s="7" t="str">
+      <c r="D86" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Low_Low</v>
       </c>
@@ -4507,17 +4501,17 @@
         <v>387</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="7">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A87" s="6">
         <v>28</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B87" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C87" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D87" s="7" t="str">
+      <c r="D87" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Low_Medium</v>
       </c>
@@ -4539,17 +4533,17 @@
         <v>388</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="7">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A88" s="6">
         <v>28</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B88" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D88" s="7" t="str">
+      <c r="D88" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Low_High</v>
       </c>
@@ -4571,17 +4565,17 @@
         <v>389</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="7">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A89" s="6">
         <v>28</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B89" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C89" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D89" s="7" t="str">
+      <c r="D89" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Low_Auto</v>
       </c>
@@ -4603,17 +4597,17 @@
         <v>390</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="7">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A90" s="6">
         <v>28</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B90" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C90" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D90" s="7" t="str">
+      <c r="D90" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Bottom_Low</v>
       </c>
@@ -4635,17 +4629,17 @@
         <v>391</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="7">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A91" s="6">
         <v>28</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B91" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C91" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D91" s="7" t="str">
+      <c r="D91" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Bottom_Medium</v>
       </c>
@@ -4667,17 +4661,17 @@
         <v>392</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="7">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A92" s="6">
         <v>28</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B92" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C92" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D92" s="7" t="str">
+      <c r="D92" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Bottom_High</v>
       </c>
@@ -4699,17 +4693,17 @@
         <v>393</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="7">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A93" s="6">
         <v>28</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B93" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C93" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D93" s="7" t="str">
+      <c r="D93" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Bottom_Auto</v>
       </c>
@@ -4731,17 +4725,17 @@
         <v>394</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
-      <c r="A94" s="7">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A94" s="6">
         <v>28</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B94" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="C94" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D94" s="7" t="str">
+      <c r="D94" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Auto_Low</v>
       </c>
@@ -4763,17 +4757,17 @@
         <v>395</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
-      <c r="A95" s="7">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A95" s="6">
         <v>28</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="B95" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C95" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D95" s="7" t="str">
+      <c r="D95" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Auto_Medium</v>
       </c>
@@ -4795,17 +4789,17 @@
         <v>396</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="7">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A96" s="6">
         <v>28</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="B96" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="C96" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D96" s="7" t="str">
+      <c r="D96" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Auto_High</v>
       </c>
@@ -4827,17 +4821,17 @@
         <v>397</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="7">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A97" s="6">
         <v>28</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="B97" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="C97" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D97" s="7" t="str">
+      <c r="D97" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_28_Auto_Auto</v>
       </c>
@@ -4859,17 +4853,17 @@
         <v>398</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="7">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A98" s="6">
         <v>29</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B98" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C98" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D98" s="7" t="str">
+      <c r="D98" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Top_Low</v>
       </c>
@@ -4891,17 +4885,17 @@
         <v>399</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
-      <c r="A99" s="7">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A99" s="6">
         <v>29</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="B99" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="C99" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D99" s="7" t="str">
+      <c r="D99" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Top_Medium</v>
       </c>
@@ -4923,17 +4917,17 @@
         <v>400</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="7">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A100" s="6">
         <v>29</v>
       </c>
-      <c r="B100" s="7" t="s">
+      <c r="B100" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D100" s="7" t="str">
+      <c r="D100" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Top_High</v>
       </c>
@@ -4955,17 +4949,17 @@
         <v>401</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
-      <c r="A101" s="7">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A101" s="6">
         <v>29</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B101" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="C101" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D101" s="7" t="str">
+      <c r="D101" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Top_Auto</v>
       </c>
@@ -4987,17 +4981,17 @@
         <v>402</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
-      <c r="A102" s="7">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A102" s="6">
         <v>29</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B102" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="7" t="s">
+      <c r="C102" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D102" s="7" t="str">
+      <c r="D102" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_High_Low</v>
       </c>
@@ -5019,17 +5013,17 @@
         <v>403</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
-      <c r="A103" s="7">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A103" s="6">
         <v>29</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B103" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C103" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D103" s="7" t="str">
+      <c r="D103" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_High_Medium</v>
       </c>
@@ -5051,17 +5045,17 @@
         <v>404</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
-      <c r="A104" s="7">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A104" s="6">
         <v>29</v>
       </c>
-      <c r="B104" s="7" t="s">
+      <c r="B104" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C104" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D104" s="7" t="str">
+      <c r="D104" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_High_High</v>
       </c>
@@ -5083,17 +5077,17 @@
         <v>405</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
-      <c r="A105" s="7">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A105" s="6">
         <v>29</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="B105" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C105" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D105" s="7" t="str">
+      <c r="D105" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_High_Auto</v>
       </c>
@@ -5115,17 +5109,17 @@
         <v>406</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
-      <c r="A106" s="7">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A106" s="6">
         <v>29</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B106" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C106" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D106" s="7" t="str">
+      <c r="D106" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Mid_Low</v>
       </c>
@@ -5147,17 +5141,17 @@
         <v>407</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
-      <c r="A107" s="7">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A107" s="6">
         <v>29</v>
       </c>
-      <c r="B107" s="7" t="s">
+      <c r="B107" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D107" s="7" t="str">
+      <c r="D107" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Mid_Medium</v>
       </c>
@@ -5179,17 +5173,17 @@
         <v>408</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
-      <c r="A108" s="7">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A108" s="6">
         <v>29</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="B108" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C108" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D108" s="7" t="str">
+      <c r="D108" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Mid_High</v>
       </c>
@@ -5211,17 +5205,17 @@
         <v>409</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
-      <c r="A109" s="7">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A109" s="6">
         <v>29</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="B109" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C109" s="7" t="s">
+      <c r="C109" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D109" s="7" t="str">
+      <c r="D109" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Mid_Auto</v>
       </c>
@@ -5243,17 +5237,17 @@
         <v>410</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
-      <c r="A110" s="7">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A110" s="6">
         <v>29</v>
       </c>
-      <c r="B110" s="7" t="s">
+      <c r="B110" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C110" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D110" s="7" t="str">
+      <c r="D110" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Low_Low</v>
       </c>
@@ -5275,17 +5269,17 @@
         <v>411</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
-      <c r="A111" s="7">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A111" s="6">
         <v>29</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B111" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C111" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D111" s="7" t="str">
+      <c r="D111" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Low_Medium</v>
       </c>
@@ -5307,17 +5301,17 @@
         <v>412</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
-      <c r="A112" s="7">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A112" s="6">
         <v>29</v>
       </c>
-      <c r="B112" s="7" t="s">
+      <c r="B112" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="C112" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D112" s="7" t="str">
+      <c r="D112" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Low_High</v>
       </c>
@@ -5339,17 +5333,17 @@
         <v>413</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
-      <c r="A113" s="7">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A113" s="6">
         <v>29</v>
       </c>
-      <c r="B113" s="7" t="s">
+      <c r="B113" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="C113" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D113" s="7" t="str">
+      <c r="D113" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Low_Auto</v>
       </c>
@@ -5371,17 +5365,17 @@
         <v>414</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
-      <c r="A114" s="7">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A114" s="6">
         <v>29</v>
       </c>
-      <c r="B114" s="7" t="s">
+      <c r="B114" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C114" s="7" t="s">
+      <c r="C114" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D114" s="7" t="str">
+      <c r="D114" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Bottom_Low</v>
       </c>
@@ -5403,17 +5397,17 @@
         <v>415</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
-      <c r="A115" s="7">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A115" s="6">
         <v>29</v>
       </c>
-      <c r="B115" s="7" t="s">
+      <c r="B115" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C115" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D115" s="7" t="str">
+      <c r="D115" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Bottom_Medium</v>
       </c>
@@ -5435,17 +5429,17 @@
         <v>416</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
-      <c r="A116" s="7">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A116" s="6">
         <v>29</v>
       </c>
-      <c r="B116" s="7" t="s">
+      <c r="B116" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C116" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D116" s="7" t="str">
+      <c r="D116" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Bottom_High</v>
       </c>
@@ -5467,17 +5461,17 @@
         <v>417</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
-      <c r="A117" s="7">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A117" s="6">
         <v>29</v>
       </c>
-      <c r="B117" s="7" t="s">
+      <c r="B117" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C117" s="7" t="s">
+      <c r="C117" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D117" s="7" t="str">
+      <c r="D117" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Bottom_Auto</v>
       </c>
@@ -5499,17 +5493,17 @@
         <v>418</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
-      <c r="A118" s="7">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A118" s="6">
         <v>29</v>
       </c>
-      <c r="B118" s="7" t="s">
+      <c r="B118" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="C118" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D118" s="7" t="str">
+      <c r="D118" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Auto_Low</v>
       </c>
@@ -5531,17 +5525,17 @@
         <v>419</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
-      <c r="A119" s="7">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A119" s="6">
         <v>29</v>
       </c>
-      <c r="B119" s="7" t="s">
+      <c r="B119" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D119" s="7" t="str">
+      <c r="D119" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Auto_Medium</v>
       </c>
@@ -5563,17 +5557,17 @@
         <v>420</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
-      <c r="A120" s="7">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A120" s="6">
         <v>29</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="B120" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C120" s="7" t="s">
+      <c r="C120" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D120" s="7" t="str">
+      <c r="D120" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Auto_High</v>
       </c>
@@ -5595,17 +5589,17 @@
         <v>421</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
-      <c r="A121" s="7">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A121" s="6">
         <v>29</v>
       </c>
-      <c r="B121" s="7" t="s">
+      <c r="B121" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="C121" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D121" s="7" t="str">
+      <c r="D121" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_29_Auto_Auto</v>
       </c>
@@ -5627,17 +5621,17 @@
         <v>422</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
-      <c r="A122" s="7">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A122" s="6">
         <v>30</v>
       </c>
-      <c r="B122" s="7" t="s">
+      <c r="B122" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C122" s="7" t="s">
+      <c r="C122" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D122" s="7" t="str">
+      <c r="D122" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_30_Top_Low</v>
       </c>
@@ -5659,17 +5653,17 @@
         <v>423</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
-      <c r="A123" s="7">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A123" s="6">
         <v>30</v>
       </c>
-      <c r="B123" s="7" t="s">
+      <c r="B123" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C123" s="7" t="s">
+      <c r="C123" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D123" s="7" t="str">
+      <c r="D123" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_30_Top_Medium</v>
       </c>
@@ -5691,17 +5685,17 @@
         <v>424</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
-      <c r="A124" s="7">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A124" s="6">
         <v>30</v>
       </c>
-      <c r="B124" s="7" t="s">
+      <c r="B124" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C124" s="7" t="s">
+      <c r="C124" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D124" s="7" t="str">
+      <c r="D124" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_30_Top_High</v>
       </c>
@@ -5723,17 +5717,17 @@
         <v>425</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
-      <c r="A125" s="7">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A125" s="6">
         <v>30</v>
       </c>
-      <c r="B125" s="7" t="s">
+      <c r="B125" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C125" s="7" t="s">
+      <c r="C125" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D125" s="7" t="str">
+      <c r="D125" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_30_Top_Auto</v>
       </c>
@@ -5755,17 +5749,17 @@
         <v>426</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
-      <c r="A126" s="7">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A126" s="6">
         <v>30</v>
       </c>
-      <c r="B126" s="7" t="s">
+      <c r="B126" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C126" s="7" t="s">
+      <c r="C126" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D126" s="7" t="str">
+      <c r="D126" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_30_High_Low</v>
       </c>
@@ -5787,17 +5781,17 @@
         <v>427</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
-      <c r="A127" s="7">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A127" s="6">
         <v>30</v>
       </c>
-      <c r="B127" s="7" t="s">
+      <c r="B127" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C127" s="7" t="s">
+      <c r="C127" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D127" s="7" t="str">
+      <c r="D127" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_30_High_Medium</v>
       </c>
@@ -5819,17 +5813,17 @@
         <v>428</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
-      <c r="A128" s="7">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A128" s="6">
         <v>30</v>
       </c>
-      <c r="B128" s="7" t="s">
+      <c r="B128" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C128" s="7" t="s">
+      <c r="C128" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D128" s="7" t="str">
+      <c r="D128" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_30_High_High</v>
       </c>
@@ -5851,17 +5845,17 @@
         <v>429</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
-      <c r="A129" s="7">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A129" s="6">
         <v>30</v>
       </c>
-      <c r="B129" s="7" t="s">
+      <c r="B129" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C129" s="7" t="s">
+      <c r="C129" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D129" s="7" t="str">
+      <c r="D129" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_30_High_Auto</v>
       </c>
@@ -5883,17 +5877,17 @@
         <v>430</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
-      <c r="A130" s="7">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A130" s="6">
         <v>30</v>
       </c>
-      <c r="B130" s="7" t="s">
+      <c r="B130" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="7" t="s">
+      <c r="C130" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D130" s="7" t="str">
+      <c r="D130" s="6" t="str">
         <f t="shared" si="3"/>
         <v>_30_Mid_Low</v>
       </c>
@@ -5915,17 +5909,17 @@
         <v>431</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
-      <c r="A131" s="7">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A131" s="6">
         <v>30</v>
       </c>
-      <c r="B131" s="7" t="s">
+      <c r="B131" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C131" s="7" t="s">
+      <c r="C131" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D131" s="7" t="str">
+      <c r="D131" s="6" t="str">
         <f t="shared" ref="D131:D145" si="6">CONCATENATE("_",A131,"_",B131,"_",C131)</f>
         <v>_30_Mid_Medium</v>
       </c>
@@ -5940,24 +5934,24 @@
         <v>288</v>
       </c>
       <c r="H131" s="1" t="str">
-        <f t="shared" ref="H131:I145" si="8">CONCATENATE("{",$H$1,D131,$H$1,", ",D131,"},")</f>
+        <f t="shared" ref="H131:H145" si="8">CONCATENATE("{",$H$1,D131,$H$1,", ",D131,"},")</f>
         <v>{"_30_Mid_Medium", _30_Mid_Medium},</v>
       </c>
       <c r="I131" s="1" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
-      <c r="A132" s="7">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A132" s="6">
         <v>30</v>
       </c>
-      <c r="B132" s="7" t="s">
+      <c r="B132" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C132" s="7" t="s">
+      <c r="C132" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D132" s="7" t="str">
+      <c r="D132" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Mid_High</v>
       </c>
@@ -5979,17 +5973,17 @@
         <v>433</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
-      <c r="A133" s="7">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A133" s="6">
         <v>30</v>
       </c>
-      <c r="B133" s="7" t="s">
+      <c r="B133" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C133" s="7" t="s">
+      <c r="C133" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D133" s="7" t="str">
+      <c r="D133" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Mid_Auto</v>
       </c>
@@ -6011,17 +6005,17 @@
         <v>434</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
-      <c r="A134" s="7">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A134" s="6">
         <v>30</v>
       </c>
-      <c r="B134" s="7" t="s">
+      <c r="B134" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C134" s="7" t="s">
+      <c r="C134" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D134" s="7" t="str">
+      <c r="D134" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Low_Low</v>
       </c>
@@ -6043,17 +6037,17 @@
         <v>435</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
-      <c r="A135" s="7">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A135" s="6">
         <v>30</v>
       </c>
-      <c r="B135" s="7" t="s">
+      <c r="B135" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C135" s="7" t="s">
+      <c r="C135" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D135" s="7" t="str">
+      <c r="D135" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Low_Medium</v>
       </c>
@@ -6075,17 +6069,17 @@
         <v>436</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
-      <c r="A136" s="7">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A136" s="6">
         <v>30</v>
       </c>
-      <c r="B136" s="7" t="s">
+      <c r="B136" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C136" s="7" t="s">
+      <c r="C136" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D136" s="7" t="str">
+      <c r="D136" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Low_High</v>
       </c>
@@ -6107,17 +6101,17 @@
         <v>437</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
-      <c r="A137" s="7">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A137" s="6">
         <v>30</v>
       </c>
-      <c r="B137" s="7" t="s">
+      <c r="B137" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C137" s="7" t="s">
+      <c r="C137" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D137" s="7" t="str">
+      <c r="D137" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Low_Auto</v>
       </c>
@@ -6139,17 +6133,17 @@
         <v>438</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
-      <c r="A138" s="7">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A138" s="6">
         <v>30</v>
       </c>
-      <c r="B138" s="7" t="s">
+      <c r="B138" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C138" s="7" t="s">
+      <c r="C138" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D138" s="7" t="str">
+      <c r="D138" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Bottom_Low</v>
       </c>
@@ -6171,17 +6165,17 @@
         <v>439</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
-      <c r="A139" s="7">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A139" s="6">
         <v>30</v>
       </c>
-      <c r="B139" s="7" t="s">
+      <c r="B139" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C139" s="7" t="s">
+      <c r="C139" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D139" s="7" t="str">
+      <c r="D139" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Bottom_Medium</v>
       </c>
@@ -6203,17 +6197,17 @@
         <v>440</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
-      <c r="A140" s="7">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A140" s="6">
         <v>30</v>
       </c>
-      <c r="B140" s="7" t="s">
+      <c r="B140" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C140" s="7" t="s">
+      <c r="C140" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D140" s="7" t="str">
+      <c r="D140" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Bottom_High</v>
       </c>
@@ -6235,17 +6229,17 @@
         <v>441</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
-      <c r="A141" s="7">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A141" s="6">
         <v>30</v>
       </c>
-      <c r="B141" s="7" t="s">
+      <c r="B141" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C141" s="7" t="s">
+      <c r="C141" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D141" s="7" t="str">
+      <c r="D141" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Bottom_Auto</v>
       </c>
@@ -6267,17 +6261,17 @@
         <v>442</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
-      <c r="A142" s="7">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A142" s="6">
         <v>30</v>
       </c>
-      <c r="B142" s="7" t="s">
+      <c r="B142" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C142" s="7" t="s">
+      <c r="C142" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D142" s="7" t="str">
+      <c r="D142" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Auto_Low</v>
       </c>
@@ -6299,17 +6293,17 @@
         <v>443</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
-      <c r="A143" s="7">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A143" s="6">
         <v>30</v>
       </c>
-      <c r="B143" s="7" t="s">
+      <c r="B143" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C143" s="7" t="s">
+      <c r="C143" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D143" s="7" t="str">
+      <c r="D143" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Auto_Medium</v>
       </c>
@@ -6331,17 +6325,17 @@
         <v>444</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
-      <c r="A144" s="7">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A144" s="6">
         <v>30</v>
       </c>
-      <c r="B144" s="7" t="s">
+      <c r="B144" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C144" s="7" t="s">
+      <c r="C144" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D144" s="7" t="str">
+      <c r="D144" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Auto_High</v>
       </c>
@@ -6363,17 +6357,17 @@
         <v>445</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
-      <c r="A145" s="7">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A145" s="6">
         <v>30</v>
       </c>
-      <c r="B145" s="7" t="s">
+      <c r="B145" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C145" s="7" t="s">
+      <c r="C145" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D145" s="7" t="str">
+      <c r="D145" s="6" t="str">
         <f t="shared" si="6"/>
         <v>_30_Auto_Auto</v>
       </c>

</xml_diff>